<commit_message>
111 Signed-off-by: 乐浩天 <215034143@qq.com>
</commit_message>
<xml_diff>
--- a/Excel/02字典_dictionary.xlsx
+++ b/Excel/02字典_dictionary.xlsx
@@ -635,7 +635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
@@ -643,7 +643,7 @@
   <cols>
     <col min="1" max="1" width="19.88671875" style="3" customWidth="1"/>
     <col min="2" max="2" width="24.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="103.88671875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="29" style="3" customWidth="1"/>
     <col min="4" max="4" width="97" style="3" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="3"/>
   </cols>

</xml_diff>